<commit_message>
Fix XLSForm compatibility issues for KoboToolbox
- Change begin_group/end_group to "begin group"/"end group" with spaces
- Replace acknowledge question type with select_one yes_only
- Add yes_only choice list for agreement questions
- Regenerate ds4owd_precourse_survey.xlsx with fixes
- Form should now upload successfully to KoboToolbox

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/ds4owd_precourse_survey.xlsx
+++ b/ds4owd_precourse_survey.xlsx
@@ -2442,7 +2442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D331"/>
+  <dimension ref="A1:D332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9070,6 +9070,26 @@
       </c>
       <c r="D331" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>yes_only</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix XLSForm CSV structure for KoboToolbox compatibility
- Add 'notes' column to match trailing commas in CSV rows
- Fix column count mismatch (21 header vs 22 data columns)
- Ensure proper CSV structure with begin group/end group syntax
- Add debugging scripts for CSV validation
- Regenerate ds4owd_precourse_survey.xlsx with correct structure

The XLSForm should now upload successfully to KoboToolbox.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/ds4owd_precourse_survey.xlsx
+++ b/ds4owd_precourse_survey.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U56"/>
+  <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,19 +541,28 @@
           <t>body::jr:requiredMsg</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>begin group</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>personal_info</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Personal Information</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -572,29 +581,34 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>github_username</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Please provide your GitHub username</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>This field is required</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -611,41 +625,46 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>orcid_id</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Please provide your ORCID iD (e.g. 0000-0003-2196-5015)</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>This field is required</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
         <is>
           <t>regex(., '^[0-9]{4}-[0-9]{4}-[0-9]{4}-[0-9]{3}[0-9X]$')</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Please enter a valid ORCID iD format</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -658,41 +677,46 @@
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>email</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Your email address</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>This field is required</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>regex(., '^[^@]+@[^@]+\.[^@]+$')</t>
-        </is>
-      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
+          <t>regex(., '^[^@]+@[^@]+.[^@]+$')</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>Please enter a valid email address</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -705,29 +729,34 @@
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>first_name</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>First Name</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>This field is required</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
@@ -744,29 +773,34 @@
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>surname</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Surname</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>This field is required</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
@@ -783,24 +817,29 @@
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>select_one countries</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>country_residence</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Country of Residence</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
@@ -818,9 +857,14 @@
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>end group</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -841,19 +885,24 @@
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>begin group</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>education_employment</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Education and Employment</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
@@ -872,24 +921,29 @@
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>select_one education_level</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>education</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Education Level</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
@@ -907,24 +961,29 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>select_one employment_status</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>employment_situation</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>What is your current employment situation?</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
@@ -942,31 +1001,36 @@
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>organisation_name</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>If employed or self-employed what is the name of the organisation / instituiton?</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
         <is>
           <t>${employment_situation}='employed_fulltime' or ${employment_situation}='employed_parttime' or ${employment_situation}='self_employed'</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -981,31 +1045,36 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>select_one organisation_type</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>org_type</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>If employed or self-employed what best describes the organisation you work for?</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
         <is>
           <t>${employment_situation}='employed_fulltime' or ${employment_situation}='employed_parttime' or ${employment_situation}='self_employed'</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
@@ -1020,9 +1089,14 @@
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>end group</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
@@ -1043,19 +1117,24 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>begin group</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>barriers</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Barriers to Participation</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
@@ -1074,19 +1153,24 @@
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>barriers_intro</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Which of the following barriers apply to your complete participation in this course?</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
@@ -1105,24 +1189,29 @@
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>select_one barrier_scale</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>barrier_time</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Time availability</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
@@ -1140,24 +1229,29 @@
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>select_one barrier_scale</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>barrier_supervisor</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>My supervisors interests</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -1175,24 +1269,29 @@
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>select_one barrier_scale</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>barrier_internet</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Access to stable internet</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
@@ -1210,24 +1309,29 @@
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>select_one barrier_scale</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>barrier_electricity</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>Access to electricity</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
@@ -1245,24 +1349,29 @@
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>select_one barrier_scale</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>barrier_computer</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>Access to computer/laptop</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
@@ -1280,24 +1389,29 @@
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>select_one barrier_scale</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>barrier_screen</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>Access to second external screen</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
@@ -1315,9 +1429,14 @@
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>end group</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
@@ -1338,19 +1457,24 @@
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>begin group</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>technical_experience</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Technical Experience</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
@@ -1369,24 +1493,29 @@
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>select_one programming_exp</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>prog_general</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>Experience with programming in general</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
@@ -1404,24 +1533,29 @@
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>select_one programming_exp</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>prog_r</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>Experience with programming in R</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
@@ -1439,24 +1573,29 @@
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>select_one programming_exp</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>prog_python</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>Experience with programming in Python</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -1474,35 +1613,40 @@
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>select_multiple prog_languages</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>other_languages</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>Which other programming languages / software do you have experience in?</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr">
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
         <is>
           <t>appearance</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
@@ -1513,24 +1657,29 @@
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>select_one git_exp</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>git_experience</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>Which of these best describes your experience with using Git?</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
@@ -1548,24 +1697,29 @@
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>select_one github_exp</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>github_experience</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>Which of these best describes your experience with using GitHub?</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -1583,24 +1737,29 @@
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>select_one data_storage</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>data_format</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>In which format do you store the majority of your data?</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -1618,24 +1777,29 @@
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>select_one doc_writing</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>narrative_docs</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>Which of these best describes how you write narrative documents that include text and analysis?</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
@@ -1653,35 +1817,40 @@
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>select_multiple ide_list</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>ide_used</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>Which of the following Integrated Development Environments (IDEs) have you used?</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr">
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
         <is>
           <t>appearance</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
@@ -1692,24 +1861,29 @@
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>select_one ide_exp</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>ide_experience</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>Which of these best describes your experience with using IDEs?</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
@@ -1727,24 +1901,29 @@
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>select_one cli_exp</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>cli_usage</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>Which of these best describes your current usage of the default command-line interface?</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
@@ -1762,35 +1941,40 @@
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>select_multiple llm_tools</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>llm_platforms</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>Which Large Language Model tools/platforms have you used?</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr">
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
         <is>
           <t>appearance</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
@@ -1801,19 +1985,24 @@
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>llm_usage_intro</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>How frequently do you use Large Language Models for the following tasks?</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
@@ -1832,24 +2021,29 @@
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>select_one llm_freq</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>llm_summarization</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>Summarization</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -1867,24 +2061,29 @@
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>select_one llm_freq</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>llm_translation</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>Translation</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
@@ -1902,24 +2101,29 @@
       <c r="S40" t="inlineStr"/>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>select_one llm_freq</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>llm_qa</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>Question Answering</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
@@ -1937,24 +2141,29 @@
       <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>select_one llm_freq</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>llm_conversation</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>Conversational Assistance</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
@@ -1972,24 +2181,29 @@
       <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>select_one llm_freq</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>llm_data_analysis</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>Data Analysis/Extraction</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
@@ -2007,24 +2221,29 @@
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>select_one llm_freq</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>llm_content_gen</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>Content Generation (e.g. images, videos)</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
@@ -2042,24 +2261,29 @@
       <c r="S44" t="inlineStr"/>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>select_one llm_freq</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>llm_learning</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>Learning/Teaching/Tutoring</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr"/>
@@ -2077,24 +2301,29 @@
       <c r="S45" t="inlineStr"/>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>select_one llm_freq</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>llm_automation</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>Agentic Task Automation</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr"/>
@@ -2112,9 +2341,14 @@
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>end group</t>
+        </is>
+      </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
@@ -2135,19 +2369,24 @@
       <c r="S47" t="inlineStr"/>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>begin group</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
           <t>project_participation</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>Project and Course Participation</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
@@ -2166,35 +2405,40 @@
       <c r="S48" t="inlineStr"/>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
           <t>learning_goals</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>What do you want to know or be able to do that you don't know or can't do right now?</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr">
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
         <is>
           <t>paragraph</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr"/>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr"/>
@@ -2205,24 +2449,29 @@
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>select_one data_available</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>data_availability</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>Can you identify a dataset of your own or your organisation that you can use for the capstone project report and share publicly as open data (see details in survey description Step 3)?</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
@@ -2240,24 +2489,29 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>select_one mentorship</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>mentorship_interest</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>We are launching a mentorship programme that brings together participants with different levels of experience, so they can support and learn from each other in small groups. Are you interested in joining this mentorship programme?</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>no</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
@@ -2275,9 +2529,14 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr"/>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>end group</t>
+        </is>
+      </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr"/>
@@ -2298,19 +2557,24 @@
       <c r="S52" t="inlineStr"/>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>begin group</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>agreements</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>Agreements and Consent</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
@@ -2329,29 +2593,34 @@
       <c r="S53" t="inlineStr"/>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>select_one yes_only</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>code_conduct</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>I acknowledge that I have read and understood the code of conduct for this course, and I commit to complying with its guidelines and principles to ensure a respectful and ethical learning environment for all participants. Available at: https://ds4owd-002.github.io/website/code_of_conduct.html</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>You must acknowledge the Code of Conduct</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
@@ -2368,29 +2637,34 @@
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>select_one yes_only</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>data_privacy</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>I agree that by submitting this form, I consent to my data being used for course administration and management, accessed only by instructors, securely stored, not shared with third parties, anonymized for reporting, and potentially used for future research to improve the course. For reporting purposes, your personal identifiers (ORCID iD, GitHub username) will be removed from the data. The anonymized data may be used for future research, scientific publications, and analysis to improve the course.</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>yes</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>You must provide consent</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
@@ -2407,9 +2681,14 @@
       <c r="S55" t="inlineStr"/>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr"/>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>end group</t>
+        </is>
+      </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
@@ -2430,6 +2709,7 @@
       <c r="S56" t="inlineStr"/>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix CLI question multiline formatting for KoboToolbox compatibility
- Convert multiline CLI question description to single line format
- Preserve all content about Mac Terminal/Zsh and Windows Terminal options
- Fix CSV structure where CLI and LLM questions were accidentally merged
- Regenerate ds4owd_precourse_survey.xlsx with corrected formatting

Resolves ValueError: unknown type ['On Mac: The default CLI app is Terminal']

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/ds4owd_precourse_survey.xlsx
+++ b/ds4owd_precourse_survey.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V59"/>
+  <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1916,10 +1916,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>"Which of these best describes your current usage of the default command-line interface (CLI)?</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
+          <t>Which of these best describes your current usage of the default command-line interface (CLI)? On Mac: The default CLI app is Terminal and the default shell is Zsh (you may also use Bash or other shells). On Windows: The default CLI app is Windows Terminal which can run Command Prompt PowerShell and Bash (via Windows Subsystem for Linux). How would you describe your experience?</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
@@ -1942,23 +1946,35 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>On Mac: The default CLI app is Terminal</t>
+          <t>select_multiple llm_tools</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> and the default shell is Zsh (you may also use Bash or other shells)</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr"/>
+          <t>llm_platforms</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Which Large Language Model tools/platforms have you used?</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>appearance</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
@@ -1974,24 +1990,20 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>On Windows: The default CLI app is Windows Terminal</t>
+          <t>note</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> which can run Command Prompt</t>
+          <t>llm_usage_intro</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PowerShell</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> and Bash (via Windows Subsystem for Linux)</t>
-        </is>
-      </c>
+          <t>How frequently do you use Large Language Models for the following tasks?</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
@@ -2014,16 +2026,24 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>How would you describe your experience?"</t>
+          <t>select_one llm_freq</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>llm_summarization</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>For Summarization (e.g., "Summarize this research paper in 200 words.")</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t>no</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
@@ -2046,17 +2066,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>select_multiple llm_tools</t>
+          <t>select_one llm_freq</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>llm_platforms</t>
+          <t>llm_translation</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Which Large Language Model tools/platforms have you used?</t>
+          <t>Translation (e.g., "Translate this email from English to German.")</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2070,11 +2090,7 @@
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>appearance</t>
-        </is>
-      </c>
+      <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
@@ -2090,20 +2106,24 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>note</t>
+          <t>select_one llm_freq</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>llm_usage_intro</t>
+          <t>llm_qa</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>How frequently do you use Large Language Models for the following tasks?</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr"/>
+          <t>Question Answering (e.g., "What are the symptoms of vitamin D deficiency?")</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
@@ -2131,12 +2151,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>llm_summarization</t>
+          <t>llm_conversation</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>For Summarization (e.g., "Summarize this research paper in 200 words.")</t>
+          <t>Conversational Assistance / Chatbots (e.g., "Help me with my online order")</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2171,12 +2191,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>llm_translation</t>
+          <t>llm_data_analysis</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Translation (e.g., "Translate this email from English to German.")</t>
+          <t>Data Analysis / Extraction (e.g., "Extract all dates and names from this contract.")</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2211,12 +2231,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>llm_qa</t>
+          <t>llm_content_gen</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Question Answering (e.g., "What are the symptoms of vitamin D deficiency?")</t>
+          <t>Content Generation (e.g. images, videos)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2251,12 +2271,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>llm_conversation</t>
+          <t>llm_learning</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Conversational Assistance / Chatbots (e.g., "Help me with my online order")</t>
+          <t>Learning/Teaching/Tutoring (e.g., "Explain the Pythagorean theorem.")</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2291,12 +2311,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>llm_data_analysis</t>
+          <t>llm_automation</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Data Analysis / Extraction (e.g., "Extract all dates and names from this contract.")</t>
+          <t>Agentic Task Automation (i.e. LLM acts autonomously or semi-autonomously to perform tasks)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2326,24 +2346,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>select_one llm_freq</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>llm_content_gen</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Content Generation (e.g. images, videos)</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+          <t>end group</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
@@ -2366,24 +2374,20 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>select_one llm_freq</t>
+          <t>begin group</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>llm_learning</t>
+          <t>project_participation</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Learning/Teaching/Tutoring (e.g., "Explain the Pythagorean theorem.")</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+          <t>Project and Course Participation</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
@@ -2406,17 +2410,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>select_one llm_freq</t>
+          <t>text</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>llm_automation</t>
+          <t>learning_goals</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Agentic Task Automation (i.e. LLM acts autonomously or semi-autonomously to perform tasks)</t>
+          <t>What do you want to know or be able to do that you don't know or can't do right now?</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2430,7 +2434,11 @@
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
-      <c r="K49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>paragraph</t>
+        </is>
+      </c>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
       <c r="N49" t="inlineStr"/>
@@ -2446,12 +2454,24 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>end group</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
+          <t>select_one data_available</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>data_availability</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Can you identify a dataset of your own or your organisation that you can use for the capstone project report and share publicly as open data (see details in survey description Step 3)?</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
@@ -2474,20 +2494,24 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>begin group</t>
+          <t>select_one mentorship</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>project_participation</t>
+          <t>mentorship_interest</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Project and Course Participation</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
+          <t>We are launching a mentorship programme that brings together participants with different levels of experience, so they can support and learn from each other in small groups. Are you interested in joining this mentorship programme?</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
@@ -2510,35 +2534,19 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>learning_goals</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>What do you want to know or be able to do that you don't know or can't do right now?</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+          <t>end group</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>paragraph</t>
-        </is>
-      </c>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr"/>
@@ -2554,24 +2562,20 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>select_one data_available</t>
+          <t>begin group</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>data_availability</t>
+          <t>agreements</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Can you identify a dataset of your own or your organisation that you can use for the capstone project report and share publicly as open data (see details in survey description Step 3)?</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
+          <t>Agreements and Consent</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
@@ -2594,25 +2598,29 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>select_one mentorship</t>
+          <t>select_one yes_only</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>mentorship_interest</t>
+          <t>code_conduct</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>We are launching a mentorship programme that brings together participants with different levels of experience, so they can support and learn from each other in small groups. Are you interested in joining this mentorship programme?</t>
+          <t>I acknowledge that I have read and understood the code of conduct for this course, and I commit to complying with its guidelines and principles to ensure a respectful and ethical learning environment for all participants. Available at: https://ds4owd-002.github.io/website/code_of_conduct.html</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr"/>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>You must acknowledge the Code of Conduct</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
@@ -2634,13 +2642,29 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>end group</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
+          <t>select_one yes_only</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>data_privacy</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>I agree that by submitting this form, I consent to my data being used for course administration and management, accessed only by instructors, securely stored, not shared with third parties, anonymized for reporting, and potentially used for future research to improve the course. For reporting purposes, your personal identifiers (ORCID iD, GitHub username) will be removed from the data. The anonymized data may be used for future research, scientific publications, and analysis to improve the course.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>You must provide consent</t>
+        </is>
+      </c>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
@@ -2662,19 +2686,11 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>begin group</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>agreements</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Agreements and Consent</t>
-        </is>
-      </c>
+          <t>end group</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr"/>
@@ -2694,122 +2710,6 @@
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>select_one yes_only</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>code_conduct</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>I acknowledge that I have read and understood the code of conduct for this course, and I commit to complying with its guidelines and principles to ensure a respectful and ethical learning environment for all participants. Available at: https://ds4owd-002.github.io/website/code_of_conduct.html</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>You must acknowledge the Code of Conduct</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
-      <c r="J57" t="inlineStr"/>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
-      <c r="N57" t="inlineStr"/>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
-      <c r="S57" t="inlineStr"/>
-      <c r="T57" t="inlineStr"/>
-      <c r="U57" t="inlineStr"/>
-      <c r="V57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>select_one yes_only</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>data_privacy</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>I agree that by submitting this form, I consent to my data being used for course administration and management, accessed only by instructors, securely stored, not shared with third parties, anonymized for reporting, and potentially used for future research to improve the course. For reporting purposes, your personal identifiers (ORCID iD, GitHub username) will be removed from the data. The anonymized data may be used for future research, scientific publications, and analysis to improve the course.</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>You must provide consent</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
-      <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
-      <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr"/>
-      <c r="N58" t="inlineStr"/>
-      <c r="O58" t="inlineStr"/>
-      <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr"/>
-      <c r="R58" t="inlineStr"/>
-      <c r="S58" t="inlineStr"/>
-      <c r="T58" t="inlineStr"/>
-      <c r="U58" t="inlineStr"/>
-      <c r="V58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>end group</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
-      <c r="J59" t="inlineStr"/>
-      <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr"/>
-      <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr"/>
-      <c r="O59" t="inlineStr"/>
-      <c r="P59" t="inlineStr"/>
-      <c r="Q59" t="inlineStr"/>
-      <c r="R59" t="inlineStr"/>
-      <c r="S59" t="inlineStr"/>
-      <c r="T59" t="inlineStr"/>
-      <c r="U59" t="inlineStr"/>
-      <c r="V59" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>